<commit_message>
Updated Sprint & Product Backlogs
ClickUp was also updated to reflect the changes made to these files
</commit_message>
<xml_diff>
--- a/deliverable4/Product_Backlog_RootDigital.xlsx
+++ b/deliverable4/Product_Backlog_RootDigital.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ewm25\Documents\GitHub\Root-Digital\deliverable3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\Desktop\Git Repositories\Root-Digital\deliverable4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF25FDEA-210B-475F-9B9D-1F2678AD3DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D1BD573-76F1-4622-AAA9-555FB60BAE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="915" windowWidth="12660" windowHeight="13335" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -453,8 +453,8 @@
   </sheetPr>
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -598,7 +598,7 @@
         <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F7" s="3">
         <v>3</v>
@@ -651,7 +651,9 @@
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <v>5</v>
+      </c>
       <c r="D10" s="1" t="s">
         <v>33</v>
       </c>
@@ -676,7 +678,7 @@
         <v>31</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="3">
         <v>5</v>
@@ -696,7 +698,7 @@
         <v>31</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="3">
         <v>3</v>
@@ -716,7 +718,7 @@
         <v>33</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="3">
         <v>5</v>
@@ -736,7 +738,7 @@
         <v>33</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F14" s="3">
         <v>8</v>
@@ -756,7 +758,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="3">
         <v>20</v>
@@ -776,7 +778,7 @@
         <v>31</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="3">
         <v>10</v>
@@ -796,7 +798,7 @@
         <v>31</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F17" s="3">
         <v>5</v>
@@ -816,7 +818,7 @@
         <v>32</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" s="3">
         <v>8</v>
@@ -896,7 +898,7 @@
         <v>33</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F22" s="3">
         <v>20</v>
@@ -916,7 +918,7 @@
         <v>31</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="3">
         <v>20</v>

</xml_diff>